<commit_message>
7 Sept intermittant commit
</commit_message>
<xml_diff>
--- a/data_files/wp files/21 Cohort Admissions Statistics TK_Aug22_ID_anonym_EDITED.xlsx
+++ b/data_files/wp files/21 Cohort Admissions Statistics TK_Aug22_ID_anonym_EDITED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matt/Google Drive/Warwick/PhD/Work/WBS/TK/FYWP Data Project/fywp_project/data_files/wp files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0824BEC5-9FD5-F243-A139-62D269D001DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B91CACB-40EB-F74B-8BA8-784806F54CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="500" windowWidth="24180" windowHeight="14920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -158,7 +158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,12 +171,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -209,21 +203,10 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -232,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -249,24 +232,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -277,6 +257,9 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9"/>
@@ -457,9 +440,6 @@
           <bgColor rgb="FFF22E00"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -475,7 +455,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J17" totalsRowShown="0" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J17" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:J17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="In Care?"/>
@@ -759,7 +739,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -768,7 +748,7 @@
       <c r="A1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" t="s">
         <v>33</v>
       </c>
       <c r="C1" t="s">
@@ -1116,7 +1096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19:G35"/>
     </sheetView>
   </sheetViews>
@@ -1125,7 +1105,7 @@
     <col min="1" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1670,579 +1650,579 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="14">
+      <c r="A20" s="12">
         <f>IF(A2="Yes", 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="12">
         <f>IF( OR(B2="Yes", C2="Yes"), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14">
+      <c r="C20" s="12"/>
+      <c r="D20" s="12">
         <f>IF(D2="Yes", 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="12">
         <f>IF(E2="Yes", 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="12">
         <f>IF(F2="Yes", 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="13">
         <f>J2</f>
         <v>45185232</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="14">
+      <c r="A21" s="12">
         <f t="shared" ref="A21:A35" si="0">IF(A3="Yes", 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="12">
         <f t="shared" ref="B21:B35" si="1">IF( OR(B3="Yes", C3="Yes"), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14">
+      <c r="C21" s="12"/>
+      <c r="D21" s="12">
         <f t="shared" ref="D21:E35" si="2">IF(D3="Yes", 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="E21" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="14">
+      <c r="E21" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="12">
         <f t="shared" ref="F21" si="3">IF(F3="Yes", 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="13">
         <f t="shared" ref="G21:G35" si="4">J3</f>
         <v>45080409</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="14">
+      <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E22" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="14">
+      <c r="C22" s="12"/>
+      <c r="D22" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="12">
         <f t="shared" ref="F22" si="5">IF(F4="Yes", 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="13">
         <f t="shared" si="4"/>
         <v>45169345</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="14">
+      <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="14">
+      <c r="C23" s="12"/>
+      <c r="D23" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="12">
         <f t="shared" ref="F23" si="6">IF(F5="Yes", 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23" s="13">
         <f t="shared" si="4"/>
         <v>45071485</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="14">
+      <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F24" s="14">
+      <c r="C24" s="12"/>
+      <c r="D24" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F24" s="12">
         <f t="shared" ref="F24" si="7">IF(F6="Yes", 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="13">
         <f t="shared" si="4"/>
         <v>45057772</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="14">
+      <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E25" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F25" s="14">
+      <c r="C25" s="12"/>
+      <c r="D25" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F25" s="12">
         <f t="shared" ref="F25" si="8">IF(F7="Yes", 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="13">
         <f t="shared" si="4"/>
         <v>45032693</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="14">
+      <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E26" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F26" s="14">
+      <c r="C26" s="12"/>
+      <c r="D26" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F26" s="12">
         <f t="shared" ref="F26" si="9">IF(F8="Yes", 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="13">
         <f t="shared" si="4"/>
         <v>45061533</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="14">
+      <c r="A27" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F27" s="14">
+      <c r="C27" s="12"/>
+      <c r="D27" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F27" s="12">
         <f t="shared" ref="F27" si="10">IF(F9="Yes", 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="15">
+      <c r="G27" s="13">
         <f t="shared" si="4"/>
         <v>45059615</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="14">
+      <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E28" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="14">
+      <c r="C28" s="12"/>
+      <c r="D28" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E28" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="12">
         <f t="shared" ref="F28" si="11">IF(F10="Yes", 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="15">
+      <c r="G28" s="13">
         <f t="shared" si="4"/>
         <v>45042325</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="14">
+      <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E29" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="14">
+      <c r="C29" s="12"/>
+      <c r="D29" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="12">
         <f t="shared" ref="F29" si="12">IF(F11="Yes", 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G29" s="13">
         <f t="shared" si="4"/>
         <v>45049143</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="14">
+      <c r="A30" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E30" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F30" s="14">
+      <c r="C30" s="12"/>
+      <c r="D30" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="12">
         <f t="shared" ref="F30" si="13">IF(F12="Yes", 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30" s="13">
         <f t="shared" si="4"/>
         <v>45052346</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="14">
+      <c r="A31" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E31" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="14">
+      <c r="C31" s="12"/>
+      <c r="D31" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E31" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="12">
         <f t="shared" ref="F31" si="14">IF(F13="Yes", 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="G31" s="15">
+      <c r="G31" s="13">
         <f t="shared" si="4"/>
         <v>45054547</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="14">
+      <c r="A32" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E32" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="14">
+      <c r="C32" s="12"/>
+      <c r="D32" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E32" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="12">
         <f t="shared" ref="F32" si="15">IF(F14="Yes", 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G32" s="15">
+      <c r="G32" s="13">
         <f t="shared" si="4"/>
         <v>45035731</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="14">
+      <c r="A33" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F33" s="14">
+      <c r="C33" s="12"/>
+      <c r="D33" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F33" s="12">
         <f t="shared" ref="F33" si="16">IF(F15="Yes", 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="G33" s="15">
+      <c r="G33" s="13">
         <f t="shared" si="4"/>
         <v>45039164</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="14">
+      <c r="A34" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E34" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="14">
+      <c r="C34" s="12"/>
+      <c r="D34" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E34" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="12">
         <f t="shared" ref="F34" si="17">IF(F16="Yes", 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="15">
+      <c r="G34" s="13">
         <f t="shared" si="4"/>
         <v>45050577</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="14">
+      <c r="A35" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B35" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E35" s="14">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F35" s="14">
+      <c r="C35" s="12"/>
+      <c r="D35" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F35" s="12">
         <f t="shared" ref="F35" si="18">IF(F17="Yes", 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G35" s="15">
+      <c r="G35" s="13">
         <f t="shared" si="4"/>
         <v>45059952</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="10"/>
-      <c r="G36" s="9"/>
+      <c r="A36" s="9"/>
+      <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="10"/>
+      <c r="A37" s="9"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="10"/>
+      <c r="A38" s="9"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
+      <c r="A39" s="9"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="10"/>
+      <c r="A40" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B19:C19"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:G4">
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:G3">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:G2">
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:G5">
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:G10">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:G6">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:G7">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:G10">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:G11">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:G12">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:G13">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:G14">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:G17">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>